<commit_message>
đã thêm mesage phần quan lý phòng
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>大項目</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>メールチェック</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更を成功</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更を失敗</t>
   </si>
 </sst>
 </file>
@@ -853,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1603,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1630,6 +1636,20 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <v>23</v>
+      </c>
+      <c r="B2">
+        <v>23.1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3">
+        <v>23.2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sua loi cua Lam
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
     <sheet name="メッセージ" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>大項目</t>
   </si>
@@ -84,132 +84,137 @@
     <t>詳細表示</t>
   </si>
   <si>
+    <t>会議室管理</t>
+  </si>
+  <si>
+    <t>全部表示</t>
+  </si>
+  <si>
+    <t>予約する</t>
+  </si>
+  <si>
+    <t>画面</t>
+  </si>
+  <si>
+    <t>全部の予約の情報を表す</t>
+  </si>
+  <si>
+    <t>検索</t>
+  </si>
+  <si>
+    <t>輸出</t>
+  </si>
+  <si>
+    <t>予約</t>
+  </si>
+  <si>
+    <t>CSV、excel を輸出する</t>
+  </si>
+  <si>
+    <t>テナントさんとか会議室とかステータスとか時間とかから検索する</t>
+  </si>
+  <si>
+    <t>一度とか毎週とか毎月とかチェック</t>
+  </si>
+  <si>
+    <t>入力チェック(フォーム)</t>
+  </si>
+  <si>
+    <t>キャンセル</t>
+  </si>
+  <si>
+    <t>時間をチェック</t>
+  </si>
+  <si>
+    <t>予約のステータスと会議室のステータスを変更する</t>
+  </si>
+  <si>
+    <t>金額を計算</t>
+  </si>
+  <si>
+    <t>VietToan</t>
+  </si>
+  <si>
+    <t>TuanAnh</t>
+  </si>
+  <si>
+    <t>データの並び替え</t>
+  </si>
+  <si>
+    <t>テナントさんの名前とか電話番号とかから検索する</t>
+  </si>
+  <si>
+    <t>テナントさんの全部の情報を表す</t>
+  </si>
+  <si>
+    <t>ユーザーの機能のログインが禁止します。</t>
+  </si>
+  <si>
+    <t>Lam</t>
+  </si>
+  <si>
+    <t>全部会議室の状態を表す</t>
+  </si>
+  <si>
+    <t>会議室がいつからいつまで予約されたか、予約されなかったかを表す。各会議室の設備を表す。</t>
+  </si>
+  <si>
+    <t>会議室の設備を変更することを表す</t>
+  </si>
+  <si>
+    <t>処理ID</t>
+  </si>
+  <si>
+    <t>メッセージID</t>
+  </si>
+  <si>
+    <t>内容</t>
+  </si>
+  <si>
+    <t>登録画面</t>
+  </si>
+  <si>
+    <t>テナントさんが本当かチェック</t>
+  </si>
+  <si>
+    <t>重複チェック</t>
+  </si>
+  <si>
+    <t>ログイン画面</t>
+  </si>
+  <si>
+    <t>ユーザーとパスワードが正しいかチェック</t>
+  </si>
+  <si>
+    <t>メールチェック</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更を成功</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更を失敗</t>
+  </si>
+  <si>
+    <t>テナントさんの一覧を表す</t>
+    <rPh sb="7" eb="9">
+      <t>イチラン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
     <t>削除</t>
-  </si>
-  <si>
-    <t>会議室管理</t>
-  </si>
-  <si>
-    <t>全部表示</t>
-  </si>
-  <si>
-    <t>予約する</t>
-  </si>
-  <si>
-    <t>画面</t>
-  </si>
-  <si>
-    <t>全部の予約の情報を表す</t>
-  </si>
-  <si>
-    <t>検索</t>
-  </si>
-  <si>
-    <t>輸出</t>
-  </si>
-  <si>
-    <t>予約</t>
-  </si>
-  <si>
-    <t>CSV、excel を輸出する</t>
-  </si>
-  <si>
-    <t>テナントさんとか会議室とかステータスとか時間とかから検索する</t>
-  </si>
-  <si>
-    <t>一度とか毎週とか毎月とかチェック</t>
-  </si>
-  <si>
-    <t>入力チェック(フォーム)</t>
-  </si>
-  <si>
-    <t>キャンセル</t>
-  </si>
-  <si>
-    <t>時間をチェック</t>
-  </si>
-  <si>
-    <t>予約のステータスと会議室のステータスを変更する</t>
-  </si>
-  <si>
-    <t>金額を計算</t>
-  </si>
-  <si>
-    <t>VietToan</t>
-  </si>
-  <si>
-    <t>TuanAnh</t>
-  </si>
-  <si>
-    <t>データの並び替え</t>
-  </si>
-  <si>
-    <t>テナントさんの名前とか電話番号とかから検索する</t>
-  </si>
-  <si>
-    <t>テナントさんの全部の情報を表す</t>
-  </si>
-  <si>
-    <t>テナントさんの順番を表す</t>
-  </si>
-  <si>
-    <t>ユーザーの機能のログインが禁止します。</t>
-  </si>
-  <si>
-    <t>Lam</t>
-  </si>
-  <si>
-    <t>全部会議室の状態を表す</t>
-  </si>
-  <si>
-    <t>会議室がいつからいつまで予約されたか、予約されなかったかを表す。各会議室の設備を表す。</t>
-  </si>
-  <si>
-    <t>会議室の設備を変更することを表す</t>
-  </si>
-  <si>
-    <t>処理ID</t>
-  </si>
-  <si>
-    <t>メッセージID</t>
-  </si>
-  <si>
-    <t>内容</t>
-  </si>
-  <si>
-    <t>登録画面</t>
-  </si>
-  <si>
-    <t>テナントさんが本当かチェック</t>
-  </si>
-  <si>
-    <t>重複チェック</t>
-  </si>
-  <si>
-    <t>ログイン画面</t>
-  </si>
-  <si>
-    <t>ユーザーとパスワードが正しいかチェック</t>
-  </si>
-  <si>
-    <t>メールチェック</t>
-  </si>
-  <si>
-    <t>会議室の設備の変更を成功</t>
-  </si>
-  <si>
-    <t>会議室の設備の変更を失敗</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -217,7 +222,7 @@
       <b/>
       <sz val="14"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -225,8 +230,15 @@
       <b/>
       <sz val="14"/>
       <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -857,31 +869,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ47"/>
+  <dimension ref="A1:AJ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="11" customWidth="1"/>
+    <col min="6" max="6" width="7.25" style="13" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="8" customWidth="1"/>
     <col min="8" max="8" width="7" style="8" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="11" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="11" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="11" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="8"/>
-    <col min="15" max="16384" width="9.140625" style="11"/>
+    <col min="9" max="9" width="7.125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="11" customWidth="1"/>
+    <col min="11" max="11" width="6.625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="6.25" style="11" customWidth="1"/>
+    <col min="13" max="14" width="9.125" style="8"/>
+    <col min="15" max="16384" width="9.125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="6" customFormat="1" ht="18.75">
+    <row r="1" spans="1:36" s="6" customFormat="1" ht="17.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -929,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>10</v>
@@ -973,7 +985,7 @@
       <c r="A3" s="26"/>
       <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>10</v>
@@ -1015,7 +1027,7 @@
       <c r="A4" s="26"/>
       <c r="B4" s="18"/>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>10</v>
@@ -1035,7 +1047,7 @@
       <c r="A5" s="26"/>
       <c r="B5" s="18"/>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>10</v>
@@ -1057,7 +1069,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>10</v>
@@ -1091,7 +1103,7 @@
       <c r="A7" s="26"/>
       <c r="B7" s="18"/>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>10</v>
@@ -1121,11 +1133,11 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:36" ht="30">
+    <row r="8" spans="1:36">
       <c r="A8" s="26"/>
       <c r="B8" s="40"/>
       <c r="C8" s="41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>10</v>
@@ -1159,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>10</v>
@@ -1193,7 +1205,7 @@
       <c r="A10" s="26"/>
       <c r="B10" s="40"/>
       <c r="C10" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>10</v>
@@ -1227,7 +1239,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="43" t="s">
         <v>10</v>
@@ -1259,7 +1271,7 @@
       <c r="A12" s="28"/>
       <c r="B12" s="44"/>
       <c r="C12" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>10</v>
@@ -1295,7 +1307,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1315,10 +1327,10 @@
     </row>
     <row r="14" spans="1:36">
       <c r="A14" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1338,10 +1350,10 @@
     </row>
     <row r="15" spans="1:36">
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -1359,9 +1371,9 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:36" ht="30">
+    <row r="16" spans="1:36" ht="27">
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -1384,7 +1396,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1404,7 +1416,7 @@
     </row>
     <row r="18" spans="1:26">
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1427,7 +1439,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -1445,111 +1457,114 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="21" spans="1:26">
-      <c r="B21" s="4" t="s">
+    <row r="20" spans="1:26">
+      <c r="B20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="43" customFormat="1">
+      <c r="A21" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="30">
+      <c r="B21" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="43" customFormat="1">
-      <c r="A23" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-    </row>
-    <row r="24" spans="1:26">
-      <c r="A24" s="12" t="s">
-        <v>40</v>
-      </c>
+    <row r="23" spans="1:26">
+      <c r="B23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="40.5">
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:26">
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="C26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" s="43" customFormat="1">
+      <c r="A27" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="45">
-      <c r="C26" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
-      <c r="B27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="30">
-      <c r="C28" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" s="43" customFormat="1">
-      <c r="A29" s="45" t="s">
+    <row r="29" spans="1:26">
+      <c r="C29" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="B31" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-    </row>
-    <row r="30" spans="1:26">
-      <c r="A30" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26">
-      <c r="C31" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="49" t="s">
+    </row>
+    <row r="32" spans="1:26" ht="27">
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="30">
-      <c r="C34" s="2" t="s">
-        <v>32</v>
+      <c r="C35" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:3">
@@ -1557,51 +1572,44 @@
         <v>29</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="C38" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="2:3">
-      <c r="B39" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="C40" s="2" t="s">
+      <c r="C39" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="C41" s="47" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="49" t="s">
+      <c r="C41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="C42" s="2" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="43" spans="2:3" ht="27">
       <c r="C43" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="C44" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="30">
-      <c r="C45" s="2" t="s">
+    <row r="45" spans="2:3">
+      <c r="B45" s="49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="49" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1611,26 +1619,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="78.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1641,7 +1649,7 @@
         <v>23.1</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1649,10 +1657,11 @@
         <v>23.2</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1663,8 +1672,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
đã chuyển vị trí row các message của quản lý phòng để tránh conflix
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
     <sheet name="メッセージ" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -214,7 +214,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -222,7 +222,7 @@
       <b/>
       <sz val="14"/>
       <color theme="2"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -230,13 +230,13 @@
       <b/>
       <sz val="14"/>
       <color theme="7" tint="-0.249977111117893"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -871,29 +871,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="11" customWidth="1"/>
-    <col min="6" max="6" width="7.25" style="13" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="8" customWidth="1"/>
     <col min="8" max="8" width="7" style="8" customWidth="1"/>
-    <col min="9" max="9" width="7.125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="11" customWidth="1"/>
-    <col min="11" max="11" width="6.625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="6.25" style="11" customWidth="1"/>
-    <col min="13" max="14" width="9.125" style="8"/>
-    <col min="15" max="16384" width="9.125" style="11"/>
+    <col min="9" max="9" width="7.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="11" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="11" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="8"/>
+    <col min="15" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="6" customFormat="1" ht="17.25">
+    <row r="1" spans="1:36" s="6" customFormat="1" ht="18.75">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1133,7 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" ht="30">
       <c r="A8" s="26"/>
       <c r="B8" s="40"/>
       <c r="C8" s="41" t="s">
@@ -1371,7 +1371,7 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:36" ht="27">
+    <row r="16" spans="1:36" ht="30">
       <c r="C16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1457,7 +1457,7 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="30">
       <c r="B20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="40.5">
+    <row r="24" spans="1:26" ht="45">
       <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" ht="30">
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="27">
+    <row r="32" spans="1:26" ht="30">
       <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="27">
+    <row r="43" spans="2:3" ht="30">
       <c r="C43" s="2" t="s">
         <v>36</v>
       </c>
@@ -1617,17 +1617,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.75" customWidth="1"/>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
-    <col min="3" max="3" width="78.75" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1641,22 +1641,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+    <row r="50" spans="1:3">
+      <c r="A50">
         <v>23</v>
       </c>
-      <c r="B2">
+      <c r="B50">
         <v>23.1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="B3">
+    <row r="51" spans="1:3">
+      <c r="B51">
         <v>23.2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C51" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1672,7 +1672,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Da them phan flow chart quan ly phong
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="10455" windowHeight="4785" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="19395" windowHeight="7245" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="会議室管理" sheetId="6" r:id="rId6"/>
     <sheet name="予約する" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>大項目</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>会議室がいつからいつまで予約されたか、予約されなかったかを表す。各会議室の設備を表す。</t>
-  </si>
-  <si>
-    <t>会議室の設備を変更することを表す</t>
   </si>
   <si>
     <t>処理ID</t>
@@ -189,14 +186,6 @@
   </si>
   <si>
     <t>削除</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>会議室の設備の変更が成功しました。</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>会議室の設備の変更が失敗しました。</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -238,6 +227,39 @@
   </si>
   <si>
     <t>ゆーざ情報変更</t>
+  </si>
+  <si>
+    <t>このユーザ名はすでに入っています。</t>
+  </si>
+  <si>
+    <t>あなたはテナントさんではありません。</t>
+  </si>
+  <si>
+    <t>登録が完成しました。</t>
+  </si>
+  <si>
+    <t>更新が成功しました。</t>
+  </si>
+  <si>
+    <t>メールアドレス形式が正しくないです。</t>
+  </si>
+  <si>
+    <t>このメールが見つかませんでした。</t>
+  </si>
+  <si>
+    <t>あなたのメールに新パスワードをお送りしました。</t>
+  </si>
+  <si>
+    <t>会議室の設備を変更することを提出する</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更が成功しました。</t>
+  </si>
+  <si>
+    <t>会議室の設備の変更が失敗しました。</t>
+  </si>
+  <si>
+    <t>会議室の設備を変更</t>
   </si>
 </sst>
 </file>
@@ -426,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -534,9 +556,6 @@
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -621,7 +640,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -668,7 +687,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -699,13 +718,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>11910</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
+      <xdr:rowOff>14288</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>450060</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -715,7 +734,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -723,8 +742,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11910" y="5357813"/>
-          <a:ext cx="3474244" cy="4629150"/>
+          <a:off x="11910" y="5348288"/>
+          <a:ext cx="3486150" cy="4629150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -762,7 +781,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -770,8 +789,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3774282" y="5345903"/>
-          <a:ext cx="3283744" cy="4572000"/>
+          <a:off x="3788569" y="5345903"/>
+          <a:ext cx="3295651" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,6 +803,44 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476742</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>134114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Snapshot_2012-02-24_232408.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10477500"/>
+          <a:ext cx="3524742" cy="5468114"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1078,8 +1135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1089,13 +1147,13 @@
     <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="7" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="9" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="9" style="9" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="9" customWidth="1"/>
     <col min="13" max="14" width="9.140625" style="6"/>
     <col min="15" max="16384" width="9.140625" style="9"/>
   </cols>
@@ -1104,10 +1162,10 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="15" t="s">
@@ -1147,8 +1205,8 @@
       <c r="B2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="45" t="s">
-        <v>47</v>
+      <c r="C2" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
@@ -1190,8 +1248,8 @@
     </row>
     <row r="3" spans="1:36">
       <c r="A3" s="18"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="44" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -1232,9 +1290,9 @@
     </row>
     <row r="4" spans="1:36">
       <c r="A4" s="18"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="46" t="s">
-        <v>48</v>
+      <c r="B4" s="40"/>
+      <c r="C4" s="45" t="s">
+        <v>47</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>10</v>
@@ -1252,9 +1310,9 @@
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="18"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="46" t="s">
-        <v>49</v>
+      <c r="B5" s="40"/>
+      <c r="C5" s="45" t="s">
+        <v>48</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -1272,11 +1330,11 @@
     </row>
     <row r="6" spans="1:36" s="8" customFormat="1">
       <c r="A6" s="18"/>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>50</v>
+      <c r="C6" s="46" t="s">
+        <v>49</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>10</v>
@@ -1308,8 +1366,8 @@
     </row>
     <row r="7" spans="1:36" s="7" customFormat="1">
       <c r="A7" s="18"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="44" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -1342,9 +1400,9 @@
     </row>
     <row r="8" spans="1:36" ht="30">
       <c r="A8" s="18"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="48" t="s">
-        <v>51</v>
+      <c r="B8" s="42"/>
+      <c r="C8" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>10</v>
@@ -1374,10 +1432,10 @@
     </row>
     <row r="9" spans="1:36" s="7" customFormat="1">
       <c r="A9" s="18"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="46" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="13" t="s">
@@ -1410,17 +1468,16 @@
     </row>
     <row r="10" spans="1:36">
       <c r="A10" s="18"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="48" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="26"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -1442,9 +1499,9 @@
     </row>
     <row r="11" spans="1:36">
       <c r="A11" s="18"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="45" t="s">
-        <v>63</v>
+      <c r="B11" s="40"/>
+      <c r="C11" s="44" t="s">
+        <v>60</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>10</v>
@@ -1474,10 +1531,10 @@
     </row>
     <row r="12" spans="1:36">
       <c r="A12" s="18"/>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="31" t="s">
@@ -1509,8 +1566,8 @@
     <row r="13" spans="1:36" s="10" customFormat="1">
       <c r="A13" s="8"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="46" t="s">
-        <v>52</v>
+      <c r="C13" s="45" t="s">
+        <v>51</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>10</v>
@@ -1543,8 +1600,8 @@
     <row r="14" spans="1:36" s="21" customFormat="1">
       <c r="A14" s="20"/>
       <c r="B14" s="32"/>
-      <c r="C14" s="50" t="s">
-        <v>64</v>
+      <c r="C14" s="49" t="s">
+        <v>61</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>10</v>
@@ -1578,10 +1635,10 @@
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="10"/>
@@ -1606,8 +1663,8 @@
         <v>40</v>
       </c>
       <c r="B16" s="36"/>
-      <c r="C16" s="46" t="s">
-        <v>53</v>
+      <c r="C16" s="45" t="s">
+        <v>52</v>
       </c>
       <c r="D16" s="10"/>
       <c r="J16" s="6"/>
@@ -1627,10 +1684,10 @@
       <c r="Z16" s="6"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="10"/>
@@ -1652,8 +1709,8 @@
     </row>
     <row r="18" spans="1:26">
       <c r="B18" s="36"/>
-      <c r="C18" s="51" t="s">
-        <v>59</v>
+      <c r="C18" s="50" t="s">
+        <v>56</v>
       </c>
       <c r="D18" s="10"/>
       <c r="J18" s="6"/>
@@ -1673,10 +1730,10 @@
       <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="10"/>
@@ -1698,8 +1755,8 @@
     </row>
     <row r="20" spans="1:26">
       <c r="B20" s="36"/>
-      <c r="C20" s="46" t="s">
-        <v>58</v>
+      <c r="C20" s="45" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="10"/>
       <c r="J20" s="6"/>
@@ -1719,10 +1776,10 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="45" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="10"/>
@@ -1743,11 +1800,11 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="1:26" ht="30">
-      <c r="B22" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>60</v>
+      <c r="B22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="10"/>
     </row>
@@ -1755,10 +1812,10 @@
       <c r="A23" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="48" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="13"/>
@@ -1773,40 +1830,40 @@
         <v>38</v>
       </c>
       <c r="B24" s="36"/>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="45" t="s">
         <v>41</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:26" ht="45">
       <c r="B26" s="36"/>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="45" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:26" ht="30">
       <c r="B28" s="36"/>
-      <c r="C28" s="46" t="s">
-        <v>43</v>
+      <c r="C28" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -1814,10 +1871,10 @@
       <c r="A29" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="48" t="s">
         <v>25</v>
       </c>
       <c r="F29" s="13"/>
@@ -1829,137 +1886,137 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B30" s="36"/>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="45" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:26">
       <c r="B31" s="36"/>
-      <c r="C31" s="46" t="s">
+      <c r="C31" s="45" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:26">
       <c r="B32" s="36"/>
-      <c r="C32" s="46"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="10"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="10"/>
     </row>
     <row r="34" spans="2:4" ht="30">
       <c r="B34" s="36"/>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="45" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="36"/>
-      <c r="C35" s="46"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="10"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="36"/>
-      <c r="C36" s="46"/>
+      <c r="C36" s="45"/>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="45" t="s">
         <v>30</v>
       </c>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="36"/>
-      <c r="C38" s="46"/>
+      <c r="C38" s="45"/>
       <c r="D38" s="10"/>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="46" t="s">
+      <c r="C39" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D39" s="10"/>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="36"/>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="45" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="10"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="36"/>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="51" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="10"/>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="36"/>
-      <c r="C42" s="46"/>
+      <c r="C42" s="45"/>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="46" t="s">
+      <c r="C43" s="45" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="36"/>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="45" t="s">
         <v>35</v>
       </c>
       <c r="D44" s="10"/>
     </row>
     <row r="45" spans="2:4" ht="30">
       <c r="B45" s="36"/>
-      <c r="C45" s="46" t="s">
+      <c r="C45" s="45" t="s">
         <v>36</v>
       </c>
       <c r="D45" s="10"/>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="36"/>
-      <c r="C46" s="46"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="46"/>
+      <c r="C47" s="45"/>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="36"/>
-      <c r="C48" s="46"/>
+      <c r="C48" s="45"/>
       <c r="D48" s="10"/>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="36"/>
-      <c r="C49" s="46"/>
+      <c r="C49" s="45"/>
       <c r="D49" s="10"/>
     </row>
   </sheetData>
@@ -1971,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1986,13 +2043,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2003,50 +2060,123 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3">
         <v>1.2</v>
       </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4">
+        <v>1.3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="B5">
+        <v>1.4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>2.1</v>
       </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6">
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50">
-        <v>21</v>
-      </c>
-      <c r="B50">
-        <v>21.1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="B51">
-        <v>21.2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>56</v>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>3.1</v>
+      </c>
+      <c r="C10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11">
+        <v>3.2</v>
+      </c>
+      <c r="C11">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12">
+        <v>3.3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15">
+        <v>4.2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16">
+        <v>4.3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>11.1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19">
+        <v>11.2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2057,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C20:I54"/>
+  <dimension ref="C20:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2080,10 +2210,20 @@
     </row>
     <row r="54" spans="3:9">
       <c r="C54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I54" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2110,7 +2250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -2122,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Up hộ thuyết Thuyết làm phần yoyaku va cancel rồi nhé. Phần quản lý phòng của tôi có 1 hình thôi mà.
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="19395" windowHeight="7245" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="19395" windowHeight="7245" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>大項目</t>
   </si>
@@ -260,6 +260,21 @@
   </si>
   <si>
     <t>会議室の設備を変更</t>
+  </si>
+  <si>
+    <t>入力フォームが正しくないです。</t>
+  </si>
+  <si>
+    <t>予約が成功でした。</t>
+  </si>
+  <si>
+    <t>2時間前以内ですから、カンセルできない。</t>
+  </si>
+  <si>
+    <t>予約がカンセルでした。</t>
+  </si>
+  <si>
+    <t>予約をカンセル</t>
   </si>
 </sst>
 </file>
@@ -807,36 +822,122 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>476742</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>134114</xdr:rowOff>
+      <xdr:colOff>505317</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>181739</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="Snapshot_2012-02-24_232408.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Snapshot_2012-02-24_232408.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="10477500"/>
+          <a:off x="28575" y="47625"/>
           <a:ext cx="3524742" cy="5468114"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419583</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>48323</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="yoyaku.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="0"/>
+          <a:ext cx="3458058" cy="5001323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552881</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="cancel.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4171950" y="0"/>
+          <a:ext cx="3086531" cy="4324954"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1136,8 +1237,8 @@
   <dimension ref="A1:AJ49"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D29:D30"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2028,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2179,6 +2280,44 @@
         <v>71</v>
       </c>
     </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <v>16.2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25">
+        <v>17.2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2187,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C20:I85"/>
+  <dimension ref="C20:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2214,16 +2353,6 @@
       </c>
       <c r="I54" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3">
-      <c r="C82" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="3:3">
-      <c r="C85" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2251,7 +2380,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2262,28 +2391,47 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C24:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="24" spans="3:10">
+      <c r="J24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Up hộ Thuyết Đã thêm 2 flow chart của phần sankaku va keisan
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="15600" windowHeight="7245"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="15600" windowHeight="7245" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="会議室管理" sheetId="6" r:id="rId6"/>
     <sheet name="予約する" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
   <si>
     <t>大項目</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>金額を計算する</t>
+  </si>
+  <si>
+    <t>金額を報告</t>
+  </si>
+  <si>
+    <t>検索しました</t>
+  </si>
+  <si>
+    <t>入力情報が存在しない。</t>
   </si>
 </sst>
 </file>
@@ -1131,6 +1140,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>505320</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>67416</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="kennsaku.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="5619750"/>
+          <a:ext cx="3543795" cy="5306166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438552</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="keisan.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="5524500"/>
+          <a:ext cx="2876952" cy="4572638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1421,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BW43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3125,10 +3210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3278,40 +3363,70 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21">
-        <v>16.100000000000001</v>
+        <v>15.1</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="B22">
-        <v>16.2</v>
+        <v>15.2</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24">
-        <v>17.100000000000001</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="B25">
+        <v>16.2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28">
         <v>17.2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3389,7 +3504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3408,10 +3523,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C24:J28"/>
+  <dimension ref="C24:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3426,6 +3541,16 @@
         <v>27</v>
       </c>
     </row>
+    <row r="56" spans="3:10">
+      <c r="J56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10">
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
hien danh sach tenato
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="15600" windowHeight="7245" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="15600" windowHeight="7245" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="処理" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -337,7 +337,7 @@
       <b/>
       <sz val="14"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -345,13 +345,13 @@
       <b/>
       <sz val="14"/>
       <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -359,7 +359,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -367,7 +367,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -833,13 +833,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -857,8 +857,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="3552825" cy="4791075"/>
+          <a:off x="0" y="66675"/>
+          <a:ext cx="3933825" cy="4314825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1023,6 +1023,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Capture.PNG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1162050" y="342900"/>
+          <a:ext cx="4448175" cy="4314825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1062,7 +1105,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1507,26 +1550,26 @@
   <dimension ref="A1:BW43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="8" customWidth="1"/>
     <col min="6" max="6" width="9" style="10" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="8" customWidth="1"/>
+    <col min="7" max="10" width="9.125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="9.75" style="8" customWidth="1"/>
     <col min="12" max="20" width="9" style="8" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="8" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="8"/>
+    <col min="21" max="21" width="9.125" style="8" customWidth="1"/>
+    <col min="22" max="16384" width="9.125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="3" customFormat="1" ht="18.75">
+    <row r="1" spans="1:75" s="3" customFormat="1" ht="17.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3212,15 +3255,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.375" customWidth="1"/>
+    <col min="2" max="2" width="7.875" customWidth="1"/>
+    <col min="3" max="3" width="49.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3439,11 +3482,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C20:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C27" sqref="C21:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="20" spans="3:9">
       <c r="F20" s="30"/>
@@ -3480,9 +3523,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3490,13 +3535,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3504,11 +3551,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S35" sqref="S27:AJ35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
@@ -3516,6 +3563,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3525,11 +3573,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C24:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="24" spans="3:10">
       <c r="J24" t="s">
@@ -3552,6 +3600,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
gan xong^^Dinh Toan xem tn roi bao minh. sorry ae vi lam muon nha ae
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="100">
   <si>
     <t>大項目</t>
   </si>
@@ -319,6 +319,36 @@
   </si>
   <si>
     <t>入力情報が存在しない。</t>
+  </si>
+  <si>
+    <t>adminではありませんですから、あらわしません。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>adminではありませんですから、検索しません。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>adminではありませんですから、許さない</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ぜひか？</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>失敗</t>
+    <rPh sb="0" eb="2">
+      <t>シッパイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <rPh sb="0" eb="2">
+      <t>セイコウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -1024,19 +1054,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="5.PNG"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="51.PNG"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1049,8 +1079,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="800099" y="342900"/>
-          <a:ext cx="4333875" cy="4276725"/>
+          <a:off x="1047750" y="495300"/>
+          <a:ext cx="4610100" cy="4276725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="61.PNG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="4972049"/>
+          <a:ext cx="4667250" cy="4829175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>143612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="9.PNG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6943725" y="4810125"/>
+          <a:ext cx="4191000" cy="5277587"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1550,8 +1656,8 @@
   <dimension ref="A1:BW43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
@@ -3253,10 +3359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3472,17 +3578,67 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B46">
         <v>6.1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>9.1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50">
+        <v>9.4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3490,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C20:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C21:D27"/>
     </sheetView>
   </sheetViews>
@@ -3543,8 +3699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>